<commit_message>
Leave 3/9/2023 12:08 AM
</commit_message>
<xml_diff>
--- a/ANGCAYA, JENNY ROSE.xlsx
+++ b/ANGCAYA, JENNY ROSE.xlsx
@@ -1,48 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVECARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4328D8C0-383F-4B0B-ACDF-B6310F0FDDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CA937C-2BDA-4541-909F-50BD538D9058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2C4B9B69-0AD3-46D4-A495-D1BDE1D16EC6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="CONVERTION" sheetId="3" r:id="rId2"/>
+    <sheet name="2017 LEAVE BALANCE" sheetId="4" r:id="rId1"/>
+    <sheet name="2018 LEAVE BALANCE" sheetId="1" r:id="rId2"/>
+    <sheet name="CONVERTION" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="BALANCE_1" localSheetId="1">[1]!Table1[[#Headers],[BALANCE]]</definedName>
+    <definedName name="BALANCE_1" localSheetId="0">Table13[[#Headers],[BALANCE]]</definedName>
+    <definedName name="BALANCE_1" localSheetId="2">[1]!Table1[[#Headers],[BALANCE]]</definedName>
     <definedName name="BALANCE_1">Table1[[#Headers],[BALANCE]]</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$9</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'2017 LEAVE BALANCE'!$1:$9</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE BALANCE'!$1:$9</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
   <si>
     <t>PERIOD</t>
   </si>
@@ -246,6 +241,18 @@
   </si>
   <si>
     <t>12/15,21,27</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>FL(2-0-0)</t>
+  </si>
+  <si>
+    <t>11/29, 12/9</t>
+  </si>
+  <si>
+    <t>2/20,21/2023</t>
   </si>
 </sst>
 </file>
@@ -623,9 +630,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -635,17 +639,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -660,7 +667,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="30">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -888,7 +895,247 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -934,25 +1181,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D52DCCA-84C7-4E23-9F01-BAD20F9E44D8}" name="Table1" displayName="Table1" ref="A8:K130" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K109" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{29298656-164E-44DD-A190-558D78410746}" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{653A013C-2253-41B2-B51E-E0CEE6FCA4B9}" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{23618FA7-8FE1-47F3-A791-7E4F2612427B}" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{BA6D2C36-5CF4-40D7-AFDD-218AEBB26721}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{44B79BA7-06A4-4888-BFE5-96396FB13C9E}" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
+      <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
+      <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
+      <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altText="BALANCE_2"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:K67" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1A20B288-1D72-4858-B3C2-871EB9CF011E}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{16E84B2D-53AC-4AEA-B1BC-1BC1E2E9B51B}" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{A10DEDBF-F571-4518-A832-0B75654FC984}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{9E225A68-4AC2-420E-B4D1-1378612CB5CD}" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{715FA023-3759-440B-8D8E-42D3E30EC36F}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{7E55BDC4-4FFC-4009-94E5-7F3F3565D56A}" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1259,16 +1536,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FF8E2B-FA0C-43AD-94F6-3305AF75672F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K130"/>
+  <dimension ref="A2:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576" topLeftCell="A89" activePane="bottomLeft"/>
-      <selection activeCell="B4" sqref="B4:C4"/>
-      <selection pane="bottomLeft" activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3696" topLeftCell="A79" activePane="bottomLeft"/>
+      <selection activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1277,11 +1554,11 @@
     <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
@@ -1290,60 +1567,60 @@
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="50"/>
+      <c r="C2" s="49"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="51"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="51"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="50"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="54"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="50"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="51"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -1369,18 +1646,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49" t="s">
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -1426,18 +1703,18 @@
       <c r="C9" s="13"/>
       <c r="D9" s="11"/>
       <c r="E9" s="13">
-        <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>38.954000000000001</v>
+        <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])</f>
+        <v>43.5</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="13">
-        <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>88.125</v>
+        <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])</f>
+        <v>77.5</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -1454,7 +1731,7 @@
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H10" s="40"/>
@@ -1468,9 +1745,7 @@
       <c r="A11" s="41">
         <v>43101</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>46</v>
-      </c>
+      <c r="B11" s="20"/>
       <c r="C11" s="13">
         <v>1.25</v>
       </c>
@@ -1478,17 +1753,13 @@
       <c r="E11" s="9"/>
       <c r="F11" s="20"/>
       <c r="G11" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
-      </c>
-      <c r="H11" s="40">
-        <v>1</v>
-      </c>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H11" s="40"/>
       <c r="I11" s="9"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="48">
-        <v>43133</v>
-      </c>
+      <c r="K11" s="48"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="41">
@@ -1504,7 +1775,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="20"/>
       <c r="G12" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H12" s="40"/>
@@ -1526,7 +1797,7 @@
       <c r="E13" s="9"/>
       <c r="F13" s="20"/>
       <c r="G13" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H13" s="40"/>
@@ -1546,7 +1817,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="20"/>
       <c r="G14" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H14" s="40"/>
@@ -1566,7 +1837,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="20"/>
       <c r="G15" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H15" s="40"/>
@@ -1586,7 +1857,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="15"/>
       <c r="G16" s="43">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H16" s="44"/>
@@ -1606,7 +1877,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="20"/>
       <c r="G17" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H17" s="40"/>
@@ -1618,29 +1889,29 @@
       <c r="A18" s="41">
         <v>43313</v>
       </c>
-      <c r="B18" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="13"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D18" s="40"/>
       <c r="E18" s="9"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H18" s="40">
-        <v>1</v>
-      </c>
+      <c r="G18" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H18" s="40"/>
       <c r="I18" s="9"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="48">
-        <v>43313</v>
-      </c>
+      <c r="K18" s="48"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="41"/>
-      <c r="B19" s="20"/>
+      <c r="A19" s="41">
+        <v>43344</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>47</v>
+      </c>
       <c r="C19" s="13">
         <v>1.25</v>
       </c>
@@ -1648,88 +1919,102 @@
       <c r="E19" s="9"/>
       <c r="F19" s="20"/>
       <c r="G19" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H19" s="40"/>
       <c r="I19" s="9"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="20"/>
+      <c r="K19" s="48">
+        <v>43356</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="41">
-        <v>43344</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="13"/>
+        <v>43374</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D20" s="40"/>
       <c r="E20" s="9"/>
       <c r="F20" s="20"/>
-      <c r="G20" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G20" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H20" s="40"/>
       <c r="I20" s="9"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="48">
-        <v>43356</v>
-      </c>
+      <c r="K20" s="20"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="41"/>
+      <c r="A21" s="41">
+        <v>43405</v>
+      </c>
       <c r="B21" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="40"/>
+        <v>48</v>
+      </c>
+      <c r="C21" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D21" s="40">
+        <v>1</v>
+      </c>
       <c r="E21" s="9"/>
       <c r="F21" s="20"/>
-      <c r="G21" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G21" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H21" s="40"/>
       <c r="I21" s="9"/>
       <c r="J21" s="11"/>
       <c r="K21" s="48">
-        <v>43353</v>
+        <v>43427</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="41"/>
-      <c r="B22" s="20"/>
+      <c r="A22" s="41">
+        <v>43435</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="C22" s="13">
         <v>1.25</v>
       </c>
-      <c r="D22" s="40"/>
+      <c r="D22" s="40">
+        <v>3</v>
+      </c>
       <c r="E22" s="9"/>
       <c r="F22" s="20"/>
       <c r="G22" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H22" s="40"/>
       <c r="I22" s="9"/>
       <c r="J22" s="11"/>
-      <c r="K22" s="20"/>
+      <c r="K22" s="20" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="41">
-        <v>43374</v>
-      </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="D23" s="40"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="40">
+        <v>1</v>
+      </c>
       <c r="E23" s="9"/>
       <c r="F23" s="20"/>
-      <c r="G23" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G23" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H23" s="40"/>
       <c r="I23" s="9"/>
@@ -1737,31 +2022,27 @@
       <c r="K23" s="20"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="41">
-        <v>43405</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="A24" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="20"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="40">
-        <v>1</v>
-      </c>
+      <c r="D24" s="40"/>
       <c r="E24" s="9"/>
       <c r="F24" s="20"/>
       <c r="G24" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H24" s="40"/>
       <c r="I24" s="9"/>
       <c r="J24" s="11"/>
-      <c r="K24" s="48">
-        <v>43427</v>
-      </c>
+      <c r="K24" s="20"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="41"/>
+      <c r="A25" s="41">
+        <v>43466</v>
+      </c>
       <c r="B25" s="20"/>
       <c r="C25" s="13">
         <v>1.25</v>
@@ -1770,7 +2051,7 @@
       <c r="E25" s="9"/>
       <c r="F25" s="20"/>
       <c r="G25" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H25" s="40"/>
@@ -1780,42 +2061,38 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="41">
-        <v>43435</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="40">
-        <v>3</v>
-      </c>
+        <v>43497</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D26" s="40"/>
       <c r="E26" s="9"/>
       <c r="F26" s="20"/>
-      <c r="G26" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G26" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H26" s="40"/>
       <c r="I26" s="9"/>
       <c r="J26" s="11"/>
-      <c r="K26" s="20" t="s">
-        <v>50</v>
-      </c>
+      <c r="K26" s="20"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="41"/>
-      <c r="B27" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="40">
-        <v>1</v>
-      </c>
+      <c r="A27" s="41">
+        <v>43525</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D27" s="40"/>
       <c r="E27" s="9"/>
       <c r="F27" s="20"/>
-      <c r="G27" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G27" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H27" s="40"/>
       <c r="I27" s="9"/>
@@ -1823,7 +2100,9 @@
       <c r="K27" s="20"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="41"/>
+      <c r="A28" s="41">
+        <v>43556</v>
+      </c>
       <c r="B28" s="20"/>
       <c r="C28" s="13">
         <v>1.25</v>
@@ -1832,7 +2111,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="20"/>
       <c r="G28" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H28" s="40"/>
@@ -1841,17 +2120,19 @@
       <c r="K28" s="20"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="47" t="s">
-        <v>51</v>
+      <c r="A29" s="41">
+        <v>43586</v>
       </c>
       <c r="B29" s="20"/>
-      <c r="C29" s="13"/>
+      <c r="C29" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D29" s="40"/>
       <c r="E29" s="9"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G29" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H29" s="40"/>
       <c r="I29" s="9"/>
@@ -1860,7 +2141,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="41">
-        <v>43466</v>
+        <v>43617</v>
       </c>
       <c r="B30" s="20"/>
       <c r="C30" s="13">
@@ -1870,7 +2151,7 @@
       <c r="E30" s="9"/>
       <c r="F30" s="20"/>
       <c r="G30" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H30" s="40"/>
@@ -1880,9 +2161,11 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="41">
-        <v>43497</v>
-      </c>
-      <c r="B31" s="20"/>
+        <v>43647</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>47</v>
+      </c>
       <c r="C31" s="13">
         <v>1.25</v>
       </c>
@@ -1890,17 +2173,19 @@
       <c r="E31" s="9"/>
       <c r="F31" s="20"/>
       <c r="G31" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H31" s="40"/>
       <c r="I31" s="9"/>
       <c r="J31" s="11"/>
-      <c r="K31" s="20"/>
+      <c r="K31" s="48">
+        <v>43655</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="41">
-        <v>43525</v>
+        <v>43678</v>
       </c>
       <c r="B32" s="20"/>
       <c r="C32" s="13">
@@ -1910,7 +2195,7 @@
       <c r="E32" s="9"/>
       <c r="F32" s="20"/>
       <c r="G32" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H32" s="40"/>
@@ -1920,9 +2205,11 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="41">
-        <v>43556</v>
-      </c>
-      <c r="B33" s="20"/>
+        <v>43709</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>52</v>
+      </c>
       <c r="C33" s="13">
         <v>1.25</v>
       </c>
@@ -1930,17 +2217,19 @@
       <c r="E33" s="9"/>
       <c r="F33" s="20"/>
       <c r="G33" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H33" s="40"/>
       <c r="I33" s="9"/>
       <c r="J33" s="11"/>
-      <c r="K33" s="20"/>
+      <c r="K33" s="20" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="41">
-        <v>43586</v>
+        <v>43739</v>
       </c>
       <c r="B34" s="20"/>
       <c r="C34" s="13">
@@ -1950,27 +2239,33 @@
       <c r="E34" s="9"/>
       <c r="F34" s="20"/>
       <c r="G34" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H34" s="40"/>
       <c r="I34" s="9"/>
       <c r="J34" s="11"/>
-      <c r="K34" s="20"/>
+      <c r="K34" s="48">
+        <v>43788</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="41">
-        <v>43617</v>
-      </c>
-      <c r="B35" s="20"/>
+        <v>43770</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="C35" s="13">
         <v>1.25</v>
       </c>
-      <c r="D35" s="40"/>
+      <c r="D35" s="40">
+        <v>1</v>
+      </c>
       <c r="E35" s="9"/>
       <c r="F35" s="20"/>
       <c r="G35" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H35" s="40"/>
@@ -1980,38 +2275,42 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="41">
-        <v>43647</v>
+        <v>43800</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="40"/>
+        <v>54</v>
+      </c>
+      <c r="C36" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D36" s="40">
+        <v>4</v>
+      </c>
       <c r="E36" s="9"/>
       <c r="F36" s="20"/>
-      <c r="G36" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G36" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H36" s="40"/>
       <c r="I36" s="9"/>
       <c r="J36" s="11"/>
-      <c r="K36" s="48">
-        <v>43655</v>
+      <c r="K36" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="41"/>
+      <c r="A37" s="47" t="s">
+        <v>44</v>
+      </c>
       <c r="B37" s="20"/>
-      <c r="C37" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="C37" s="13"/>
       <c r="D37" s="40"/>
       <c r="E37" s="9"/>
       <c r="F37" s="20"/>
-      <c r="G37" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G37" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H37" s="40"/>
       <c r="I37" s="9"/>
@@ -2020,7 +2319,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="41">
-        <v>43678</v>
+        <v>43831</v>
       </c>
       <c r="B38" s="20"/>
       <c r="C38" s="13">
@@ -2030,38 +2329,38 @@
       <c r="E38" s="9"/>
       <c r="F38" s="20"/>
       <c r="G38" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H38" s="40"/>
       <c r="I38" s="9"/>
       <c r="J38" s="11"/>
-      <c r="K38" s="20"/>
+      <c r="K38" s="48"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="41">
-        <v>43709</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="13"/>
+        <v>43862</v>
+      </c>
+      <c r="B39" s="20"/>
+      <c r="C39" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D39" s="40"/>
       <c r="E39" s="9"/>
       <c r="F39" s="20"/>
-      <c r="G39" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G39" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H39" s="40"/>
       <c r="I39" s="9"/>
       <c r="J39" s="11"/>
-      <c r="K39" s="20" t="s">
-        <v>53</v>
-      </c>
+      <c r="K39" s="48"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="41"/>
+      <c r="A40" s="41">
+        <v>43891</v>
+      </c>
       <c r="B40" s="20"/>
       <c r="C40" s="13">
         <v>1.25</v>
@@ -2070,7 +2369,7 @@
       <c r="E40" s="9"/>
       <c r="F40" s="20"/>
       <c r="G40" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H40" s="40"/>
@@ -2080,7 +2379,8 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="41">
-        <v>43739</v>
+        <f>EDATE(A40,1)</f>
+        <v>43922</v>
       </c>
       <c r="B41" s="20"/>
       <c r="C41" s="13">
@@ -2090,32 +2390,29 @@
       <c r="E41" s="9"/>
       <c r="F41" s="20"/>
       <c r="G41" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H41" s="40"/>
       <c r="I41" s="9"/>
       <c r="J41" s="11"/>
-      <c r="K41" s="48">
-        <v>43788</v>
-      </c>
+      <c r="K41" s="20"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="41">
-        <v>43770</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="40">
-        <v>1</v>
-      </c>
+        <f t="shared" ref="A42:A45" si="0">EDATE(A41,1)</f>
+        <v>43952</v>
+      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D42" s="40"/>
       <c r="E42" s="9"/>
       <c r="F42" s="20"/>
-      <c r="G42" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G42" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H42" s="40"/>
       <c r="I42" s="9"/>
@@ -2123,7 +2420,10 @@
       <c r="K42" s="20"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="41"/>
+      <c r="A43" s="41">
+        <f t="shared" si="0"/>
+        <v>43983</v>
+      </c>
       <c r="B43" s="20"/>
       <c r="C43" s="13">
         <v>1.25</v>
@@ -2132,7 +2432,7 @@
       <c r="E43" s="9"/>
       <c r="F43" s="20"/>
       <c r="G43" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H43" s="40"/>
@@ -2142,42 +2442,40 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="41">
-        <v>43800</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>54</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>44013</v>
+      </c>
+      <c r="B44" s="20"/>
       <c r="C44" s="13">
         <v>1.25</v>
       </c>
-      <c r="D44" s="40">
-        <v>4</v>
-      </c>
+      <c r="D44" s="40"/>
       <c r="E44" s="9"/>
       <c r="F44" s="20"/>
       <c r="G44" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H44" s="40"/>
       <c r="I44" s="9"/>
       <c r="J44" s="11"/>
-      <c r="K44" s="20" t="s">
-        <v>55</v>
-      </c>
+      <c r="K44" s="20"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="47" t="s">
-        <v>44</v>
+      <c r="A45" s="41">
+        <f t="shared" si="0"/>
+        <v>44044</v>
       </c>
       <c r="B45" s="20"/>
-      <c r="C45" s="13"/>
+      <c r="C45" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D45" s="40"/>
       <c r="E45" s="9"/>
       <c r="F45" s="20"/>
-      <c r="G45" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G45" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H45" s="40"/>
       <c r="I45" s="9"/>
@@ -2186,28 +2484,28 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="41">
-        <v>43831</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="13"/>
+        <v>44075</v>
+      </c>
+      <c r="B46" s="20"/>
+      <c r="C46" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D46" s="40"/>
       <c r="E46" s="9"/>
       <c r="F46" s="20"/>
-      <c r="G46" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G46" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H46" s="40"/>
       <c r="I46" s="9"/>
       <c r="J46" s="11"/>
-      <c r="K46" s="48">
-        <v>43847</v>
-      </c>
+      <c r="K46" s="48"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="41"/>
+      <c r="A47" s="41">
+        <v>44105</v>
+      </c>
       <c r="B47" s="20"/>
       <c r="C47" s="13">
         <v>1.25</v>
@@ -2216,7 +2514,7 @@
       <c r="E47" s="9"/>
       <c r="F47" s="20"/>
       <c r="G47" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H47" s="40"/>
@@ -2226,37 +2524,41 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="41">
-        <v>43862</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" s="13"/>
+        <v>44136</v>
+      </c>
+      <c r="B48" s="20"/>
+      <c r="C48" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D48" s="40"/>
       <c r="E48" s="9"/>
       <c r="F48" s="20"/>
-      <c r="G48" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G48" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H48" s="40"/>
       <c r="I48" s="9"/>
       <c r="J48" s="11"/>
-      <c r="K48" s="48">
-        <v>43889</v>
-      </c>
+      <c r="K48" s="20"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A49" s="41"/>
-      <c r="B49" s="20"/>
+      <c r="A49" s="41">
+        <v>44166</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>57</v>
+      </c>
       <c r="C49" s="13">
         <v>1.25</v>
       </c>
-      <c r="D49" s="40"/>
+      <c r="D49" s="40">
+        <v>5</v>
+      </c>
       <c r="E49" s="9"/>
       <c r="F49" s="20"/>
       <c r="G49" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H49" s="40"/>
@@ -2265,19 +2567,17 @@
       <c r="K49" s="20"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A50" s="41">
-        <v>43891</v>
+      <c r="A50" s="47" t="s">
+        <v>58</v>
       </c>
       <c r="B50" s="20"/>
-      <c r="C50" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="C50" s="13"/>
       <c r="D50" s="40"/>
       <c r="E50" s="9"/>
       <c r="F50" s="20"/>
-      <c r="G50" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G50" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H50" s="40"/>
       <c r="I50" s="9"/>
@@ -2286,8 +2586,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="41">
-        <f>EDATE(A50,1)</f>
-        <v>43922</v>
+        <v>44197</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="13">
@@ -2297,7 +2596,7 @@
       <c r="E51" s="9"/>
       <c r="F51" s="20"/>
       <c r="G51" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H51" s="40"/>
@@ -2307,8 +2606,8 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="41">
-        <f t="shared" ref="A52:A55" si="0">EDATE(A51,1)</f>
-        <v>43952</v>
+        <f>EDATE(A51,1)</f>
+        <v>44228</v>
       </c>
       <c r="B52" s="20"/>
       <c r="C52" s="13">
@@ -2318,7 +2617,7 @@
       <c r="E52" s="9"/>
       <c r="F52" s="20"/>
       <c r="G52" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H52" s="40"/>
@@ -2328,8 +2627,8 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="41">
-        <f t="shared" si="0"/>
-        <v>43983</v>
+        <f t="shared" ref="A53:A58" si="1">EDATE(A52,1)</f>
+        <v>44256</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="13">
@@ -2339,7 +2638,7 @@
       <c r="E53" s="9"/>
       <c r="F53" s="20"/>
       <c r="G53" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H53" s="40"/>
@@ -2349,8 +2648,8 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="41">
-        <f t="shared" si="0"/>
-        <v>44013</v>
+        <f t="shared" si="1"/>
+        <v>44287</v>
       </c>
       <c r="B54" s="20"/>
       <c r="C54" s="13">
@@ -2360,7 +2659,7 @@
       <c r="E54" s="9"/>
       <c r="F54" s="20"/>
       <c r="G54" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H54" s="40"/>
@@ -2370,8 +2669,8 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="41">
-        <f t="shared" si="0"/>
-        <v>44044</v>
+        <f t="shared" si="1"/>
+        <v>44317</v>
       </c>
       <c r="B55" s="20"/>
       <c r="C55" s="13">
@@ -2381,7 +2680,7 @@
       <c r="E55" s="9"/>
       <c r="F55" s="20"/>
       <c r="G55" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H55" s="40"/>
@@ -2391,28 +2690,30 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="41">
-        <v>44075</v>
-      </c>
-      <c r="B56" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C56" s="13"/>
+        <f t="shared" si="1"/>
+        <v>44348</v>
+      </c>
+      <c r="B56" s="20"/>
+      <c r="C56" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D56" s="40"/>
       <c r="E56" s="9"/>
       <c r="F56" s="20"/>
-      <c r="G56" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G56" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H56" s="40"/>
       <c r="I56" s="9"/>
       <c r="J56" s="11"/>
-      <c r="K56" s="48">
-        <v>44088</v>
-      </c>
+      <c r="K56" s="20"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" s="41"/>
+      <c r="A57" s="41">
+        <f t="shared" si="1"/>
+        <v>44378</v>
+      </c>
       <c r="B57" s="20"/>
       <c r="C57" s="13">
         <v>1.25</v>
@@ -2421,7 +2722,7 @@
       <c r="E57" s="9"/>
       <c r="F57" s="20"/>
       <c r="G57" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H57" s="40"/>
@@ -2431,7 +2732,8 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="41">
-        <v>44105</v>
+        <f t="shared" si="1"/>
+        <v>44409</v>
       </c>
       <c r="B58" s="20"/>
       <c r="C58" s="13">
@@ -2441,7 +2743,7 @@
       <c r="E58" s="9"/>
       <c r="F58" s="20"/>
       <c r="G58" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H58" s="40"/>
@@ -2451,16 +2753,18 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="41">
-        <v>44136</v>
+        <v>44440</v>
       </c>
       <c r="B59" s="20"/>
-      <c r="C59" s="13"/>
+      <c r="C59" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D59" s="40"/>
       <c r="E59" s="9"/>
       <c r="F59" s="20"/>
-      <c r="G59" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G59" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H59" s="40"/>
       <c r="I59" s="9"/>
@@ -2469,21 +2773,17 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="41">
-        <v>44166</v>
-      </c>
-      <c r="B60" s="20" t="s">
-        <v>57</v>
-      </c>
+        <v>44470</v>
+      </c>
+      <c r="B60" s="20"/>
       <c r="C60" s="13">
         <v>1.25</v>
       </c>
-      <c r="D60" s="40">
-        <v>5</v>
-      </c>
+      <c r="D60" s="40"/>
       <c r="E60" s="9"/>
       <c r="F60" s="20"/>
       <c r="G60" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H60" s="40"/>
@@ -2492,79 +2792,91 @@
       <c r="K60" s="20"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="20"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="40"/>
+      <c r="A61" s="41">
+        <v>44501</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D61" s="40">
+        <v>5</v>
+      </c>
       <c r="E61" s="9"/>
       <c r="F61" s="20"/>
-      <c r="G61" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G61" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H61" s="40"/>
       <c r="I61" s="9"/>
       <c r="J61" s="11"/>
-      <c r="K61" s="20"/>
+      <c r="K61" s="20" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="41">
-        <v>44197</v>
-      </c>
-      <c r="B62" s="20"/>
+        <v>44531</v>
+      </c>
+      <c r="B62" s="20" t="s">
+        <v>61</v>
+      </c>
       <c r="C62" s="13">
         <v>1.25</v>
       </c>
-      <c r="D62" s="40"/>
+      <c r="D62" s="40">
+        <v>5</v>
+      </c>
       <c r="E62" s="9"/>
       <c r="F62" s="20"/>
       <c r="G62" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H62" s="40"/>
       <c r="I62" s="9"/>
       <c r="J62" s="11"/>
-      <c r="K62" s="20"/>
+      <c r="K62" s="20" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A63" s="41">
-        <f>EDATE(A62,1)</f>
-        <v>44228</v>
-      </c>
-      <c r="B63" s="20"/>
-      <c r="C63" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="D63" s="40"/>
+      <c r="A63" s="41"/>
+      <c r="B63" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" s="13"/>
+      <c r="D63" s="40">
+        <v>1</v>
+      </c>
       <c r="E63" s="9"/>
       <c r="F63" s="20"/>
-      <c r="G63" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G63" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H63" s="40"/>
       <c r="I63" s="9"/>
       <c r="J63" s="11"/>
-      <c r="K63" s="20"/>
+      <c r="K63" s="48">
+        <v>44266</v>
+      </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A64" s="41">
-        <f t="shared" ref="A64:A69" si="1">EDATE(A63,1)</f>
-        <v>44256</v>
+      <c r="A64" s="47" t="s">
+        <v>65</v>
       </c>
       <c r="B64" s="20"/>
-      <c r="C64" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="C64" s="13"/>
       <c r="D64" s="40"/>
       <c r="E64" s="9"/>
       <c r="F64" s="20"/>
-      <c r="G64" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G64" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H64" s="40"/>
       <c r="I64" s="9"/>
@@ -2573,8 +2885,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="41">
-        <f t="shared" si="1"/>
-        <v>44287</v>
+        <v>44562</v>
       </c>
       <c r="B65" s="20"/>
       <c r="C65" s="13">
@@ -2584,7 +2895,7 @@
       <c r="E65" s="9"/>
       <c r="F65" s="20"/>
       <c r="G65" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H65" s="40"/>
@@ -2594,8 +2905,8 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="41">
-        <f t="shared" si="1"/>
-        <v>44317</v>
+        <f>EDATE(A65,1)</f>
+        <v>44593</v>
       </c>
       <c r="B66" s="20"/>
       <c r="C66" s="13">
@@ -2605,7 +2916,7 @@
       <c r="E66" s="9"/>
       <c r="F66" s="20"/>
       <c r="G66" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H66" s="40"/>
@@ -2615,8 +2926,8 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="41">
-        <f t="shared" si="1"/>
-        <v>44348</v>
+        <f t="shared" ref="A67:A70" si="2">EDATE(A66,1)</f>
+        <v>44621</v>
       </c>
       <c r="B67" s="20"/>
       <c r="C67" s="13">
@@ -2626,7 +2937,7 @@
       <c r="E67" s="9"/>
       <c r="F67" s="20"/>
       <c r="G67" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H67" s="40"/>
@@ -2636,8 +2947,8 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="41">
-        <f t="shared" si="1"/>
-        <v>44378</v>
+        <f t="shared" si="2"/>
+        <v>44652</v>
       </c>
       <c r="B68" s="20"/>
       <c r="C68" s="13">
@@ -2647,7 +2958,7 @@
       <c r="E68" s="9"/>
       <c r="F68" s="20"/>
       <c r="G68" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H68" s="40"/>
@@ -2657,111 +2968,124 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="41">
-        <f t="shared" si="1"/>
-        <v>44409</v>
-      </c>
-      <c r="B69" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C69" s="13"/>
+        <f t="shared" si="2"/>
+        <v>44682</v>
+      </c>
+      <c r="B69" s="20"/>
+      <c r="C69" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D69" s="40"/>
       <c r="E69" s="9"/>
       <c r="F69" s="20"/>
-      <c r="G69" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G69" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H69" s="40"/>
       <c r="I69" s="9"/>
       <c r="J69" s="11"/>
-      <c r="K69" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="K69" s="20"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A70" s="41"/>
-      <c r="B70" s="20"/>
+      <c r="A70" s="41">
+        <f t="shared" si="2"/>
+        <v>44713</v>
+      </c>
+      <c r="B70" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="C70" s="13">
         <v>1.25</v>
       </c>
-      <c r="D70" s="40"/>
+      <c r="D70" s="40">
+        <v>1</v>
+      </c>
       <c r="E70" s="9"/>
       <c r="F70" s="20"/>
       <c r="G70" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H70" s="40"/>
       <c r="I70" s="9"/>
       <c r="J70" s="11"/>
-      <c r="K70" s="20"/>
+      <c r="K70" s="48">
+        <v>44718</v>
+      </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A71" s="41">
-        <v>44440</v>
-      </c>
-      <c r="B71" s="20"/>
-      <c r="C71" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="D71" s="40"/>
+      <c r="A71" s="41"/>
+      <c r="B71" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C71" s="13"/>
+      <c r="D71" s="40">
+        <v>1</v>
+      </c>
       <c r="E71" s="9"/>
       <c r="F71" s="20"/>
-      <c r="G71" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G71" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H71" s="40"/>
       <c r="I71" s="9"/>
       <c r="J71" s="11"/>
-      <c r="K71" s="20"/>
+      <c r="K71" s="48">
+        <v>44729</v>
+      </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="41">
-        <v>44470</v>
-      </c>
-      <c r="B72" s="20"/>
+        <v>44743</v>
+      </c>
+      <c r="B72" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="C72" s="13">
         <v>1.25</v>
       </c>
-      <c r="D72" s="40"/>
+      <c r="D72" s="40">
+        <v>1</v>
+      </c>
       <c r="E72" s="9"/>
       <c r="F72" s="20"/>
       <c r="G72" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H72" s="40"/>
       <c r="I72" s="9"/>
       <c r="J72" s="11"/>
-      <c r="K72" s="20"/>
+      <c r="K72" s="48">
+        <v>44769</v>
+      </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="41">
-        <v>44501</v>
-      </c>
-      <c r="B73" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C73" s="13"/>
-      <c r="D73" s="40">
-        <v>5</v>
-      </c>
+        <v>44774</v>
+      </c>
+      <c r="B73" s="20"/>
+      <c r="C73" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D73" s="40"/>
       <c r="E73" s="9"/>
       <c r="F73" s="20"/>
-      <c r="G73" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G73" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H73" s="40"/>
       <c r="I73" s="9"/>
       <c r="J73" s="11"/>
-      <c r="K73" s="20" t="s">
-        <v>62</v>
-      </c>
+      <c r="K73" s="48"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A74" s="41"/>
+      <c r="A74" s="41">
+        <v>44805</v>
+      </c>
       <c r="B74" s="20"/>
       <c r="C74" s="13">
         <v>1.25</v>
@@ -2770,81 +3094,89 @@
       <c r="E74" s="9"/>
       <c r="F74" s="20"/>
       <c r="G74" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H74" s="40"/>
       <c r="I74" s="9"/>
       <c r="J74" s="11"/>
-      <c r="K74" s="20"/>
+      <c r="K74" s="48"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="41">
-        <v>44531</v>
-      </c>
-      <c r="B75" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C75" s="13"/>
-      <c r="D75" s="40">
-        <v>5</v>
-      </c>
+        <v>44848</v>
+      </c>
+      <c r="B75" s="20"/>
+      <c r="C75" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D75" s="40"/>
       <c r="E75" s="9"/>
       <c r="F75" s="20"/>
-      <c r="G75" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G75" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H75" s="40"/>
       <c r="I75" s="9"/>
       <c r="J75" s="11"/>
-      <c r="K75" s="20" t="s">
-        <v>63</v>
-      </c>
+      <c r="K75" s="48"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A76" s="41"/>
+      <c r="A76" s="41">
+        <v>44866</v>
+      </c>
       <c r="B76" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C76" s="13"/>
+        <v>69</v>
+      </c>
+      <c r="C76" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D76" s="40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="20"/>
-      <c r="G76" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G76" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H76" s="40"/>
       <c r="I76" s="9"/>
       <c r="J76" s="11"/>
-      <c r="K76" s="48">
-        <v>44266</v>
+      <c r="K76" s="48" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="41"/>
-      <c r="B77" s="20"/>
+      <c r="A77" s="41">
+        <v>44896</v>
+      </c>
+      <c r="B77" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="C77" s="13">
         <v>1.25</v>
       </c>
-      <c r="D77" s="40"/>
+      <c r="D77" s="40">
+        <v>3</v>
+      </c>
       <c r="E77" s="9"/>
       <c r="F77" s="20"/>
       <c r="G77" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
       <c r="H77" s="40"/>
       <c r="I77" s="9"/>
       <c r="J77" s="11"/>
-      <c r="K77" s="20"/>
+      <c r="K77" s="20" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="47" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -2852,7 +3184,7 @@
       <c r="E78" s="9"/>
       <c r="F78" s="20"/>
       <c r="G78" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H78" s="40"/>
@@ -2862,16 +3194,18 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="41">
-        <v>44562</v>
+        <v>44927</v>
       </c>
       <c r="B79" s="20"/>
-      <c r="C79" s="13"/>
+      <c r="C79" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D79" s="40"/>
       <c r="E79" s="9"/>
       <c r="F79" s="20"/>
-      <c r="G79" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G79" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H79" s="40"/>
       <c r="I79" s="9"/>
@@ -2880,27 +3214,31 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="41">
-        <f>EDATE(A79,1)</f>
-        <v>44593</v>
-      </c>
-      <c r="B80" s="20"/>
-      <c r="C80" s="13"/>
+        <v>44958</v>
+      </c>
+      <c r="B80" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C80" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D80" s="40"/>
       <c r="E80" s="9"/>
       <c r="F80" s="20"/>
-      <c r="G80" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G80" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H80" s="40"/>
       <c r="I80" s="9"/>
       <c r="J80" s="11"/>
-      <c r="K80" s="20"/>
+      <c r="K80" s="20" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="41">
-        <f t="shared" ref="A81:A84" si="2">EDATE(A80,1)</f>
-        <v>44621</v>
+        <v>44986</v>
       </c>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -2908,7 +3246,7 @@
       <c r="E81" s="9"/>
       <c r="F81" s="20"/>
       <c r="G81" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H81" s="40"/>
@@ -2918,8 +3256,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="41">
-        <f t="shared" si="2"/>
-        <v>44652</v>
+        <v>45017</v>
       </c>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -2927,7 +3264,7 @@
       <c r="E82" s="9"/>
       <c r="F82" s="20"/>
       <c r="G82" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H82" s="40"/>
@@ -2937,8 +3274,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="41">
-        <f t="shared" si="2"/>
-        <v>44682</v>
+        <v>45047</v>
       </c>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -2946,7 +3282,7 @@
       <c r="E83" s="9"/>
       <c r="F83" s="20"/>
       <c r="G83" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H83" s="40"/>
@@ -2956,63 +3292,52 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="41">
-        <f t="shared" si="2"/>
-        <v>44713</v>
-      </c>
-      <c r="B84" s="20" t="s">
-        <v>64</v>
-      </c>
+        <v>45078</v>
+      </c>
+      <c r="B84" s="20"/>
       <c r="C84" s="13"/>
-      <c r="D84" s="40">
-        <v>1</v>
-      </c>
+      <c r="D84" s="40"/>
       <c r="E84" s="9"/>
       <c r="F84" s="20"/>
       <c r="G84" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H84" s="40"/>
       <c r="I84" s="9"/>
       <c r="J84" s="11"/>
-      <c r="K84" s="48">
-        <v>44718</v>
-      </c>
+      <c r="K84" s="20"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A85" s="41"/>
-      <c r="B85" s="20" t="s">
-        <v>64</v>
-      </c>
+      <c r="A85" s="41">
+        <v>45108</v>
+      </c>
+      <c r="B85" s="20"/>
       <c r="C85" s="13"/>
-      <c r="D85" s="40">
-        <v>1</v>
-      </c>
+      <c r="D85" s="40"/>
       <c r="E85" s="9"/>
       <c r="F85" s="20"/>
       <c r="G85" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H85" s="40"/>
       <c r="I85" s="9"/>
       <c r="J85" s="11"/>
-      <c r="K85" s="48">
-        <v>44729</v>
-      </c>
+      <c r="K85" s="20"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A86" s="41"/>
+      <c r="A86" s="41">
+        <v>45139</v>
+      </c>
       <c r="B86" s="20"/>
-      <c r="C86" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="C86" s="13"/>
       <c r="D86" s="40"/>
       <c r="E86" s="9"/>
       <c r="F86" s="20"/>
-      <c r="G86" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G86" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H86" s="40"/>
       <c r="I86" s="9"/>
@@ -3021,60 +3346,52 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="41">
-        <v>44743</v>
-      </c>
-      <c r="B87" s="20" t="s">
-        <v>47</v>
-      </c>
+        <v>45170</v>
+      </c>
+      <c r="B87" s="20"/>
       <c r="C87" s="13"/>
       <c r="D87" s="40"/>
       <c r="E87" s="9"/>
       <c r="F87" s="20"/>
       <c r="G87" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H87" s="40"/>
       <c r="I87" s="9"/>
       <c r="J87" s="11"/>
-      <c r="K87" s="48" t="s">
-        <v>66</v>
-      </c>
+      <c r="K87" s="20"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A88" s="41"/>
-      <c r="B88" s="20" t="s">
-        <v>64</v>
-      </c>
+      <c r="A88" s="41">
+        <v>45200</v>
+      </c>
+      <c r="B88" s="20"/>
       <c r="C88" s="13"/>
-      <c r="D88" s="40">
-        <v>1</v>
-      </c>
+      <c r="D88" s="40"/>
       <c r="E88" s="9"/>
       <c r="F88" s="20"/>
       <c r="G88" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H88" s="40"/>
       <c r="I88" s="9"/>
       <c r="J88" s="11"/>
-      <c r="K88" s="48">
-        <v>44769</v>
-      </c>
+      <c r="K88" s="20"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A89" s="41"/>
+      <c r="A89" s="41">
+        <v>45231</v>
+      </c>
       <c r="B89" s="20"/>
-      <c r="C89" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="C89" s="13"/>
       <c r="D89" s="40"/>
       <c r="E89" s="9"/>
       <c r="F89" s="20"/>
-      <c r="G89" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G89" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H89" s="40"/>
       <c r="I89" s="9"/>
@@ -3083,80 +3400,70 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="41">
-        <v>44774</v>
-      </c>
-      <c r="B90" s="20" t="s">
-        <v>47</v>
-      </c>
+        <v>45261</v>
+      </c>
+      <c r="B90" s="20"/>
       <c r="C90" s="13"/>
       <c r="D90" s="40"/>
       <c r="E90" s="9"/>
       <c r="F90" s="20"/>
       <c r="G90" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H90" s="40"/>
       <c r="I90" s="9"/>
       <c r="J90" s="11"/>
-      <c r="K90" s="48">
-        <v>44793</v>
-      </c>
+      <c r="K90" s="20"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A91" s="41"/>
-      <c r="B91" s="20" t="s">
-        <v>47</v>
-      </c>
+      <c r="A91" s="41">
+        <v>45292</v>
+      </c>
+      <c r="B91" s="20"/>
       <c r="C91" s="13"/>
       <c r="D91" s="40"/>
       <c r="E91" s="9"/>
       <c r="F91" s="20"/>
       <c r="G91" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H91" s="40"/>
       <c r="I91" s="9"/>
       <c r="J91" s="11"/>
-      <c r="K91" s="48">
-        <v>44774</v>
-      </c>
+      <c r="K91" s="20"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A92" s="41"/>
-      <c r="B92" s="20" t="s">
-        <v>46</v>
-      </c>
+      <c r="A92" s="41">
+        <v>45323</v>
+      </c>
+      <c r="B92" s="20"/>
       <c r="C92" s="13"/>
       <c r="D92" s="40"/>
       <c r="E92" s="9"/>
       <c r="F92" s="20"/>
       <c r="G92" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H92" s="40">
-        <v>1</v>
-      </c>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H92" s="40"/>
       <c r="I92" s="9"/>
       <c r="J92" s="11"/>
-      <c r="K92" s="48">
-        <v>44795</v>
-      </c>
+      <c r="K92" s="20"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A93" s="41"/>
+      <c r="A93" s="41">
+        <v>45352</v>
+      </c>
       <c r="B93" s="20"/>
-      <c r="C93" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="C93" s="13"/>
       <c r="D93" s="40"/>
       <c r="E93" s="9"/>
       <c r="F93" s="20"/>
-      <c r="G93" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G93" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H93" s="40"/>
       <c r="I93" s="9"/>
@@ -3165,40 +3472,34 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="41">
-        <v>44805</v>
-      </c>
-      <c r="B94" s="20" t="s">
-        <v>46</v>
-      </c>
+        <v>45383</v>
+      </c>
+      <c r="B94" s="20"/>
       <c r="C94" s="13"/>
       <c r="D94" s="40"/>
       <c r="E94" s="9"/>
       <c r="F94" s="20"/>
       <c r="G94" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H94" s="40">
-        <v>1</v>
-      </c>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H94" s="40"/>
       <c r="I94" s="9"/>
       <c r="J94" s="11"/>
-      <c r="K94" s="48">
-        <v>44820</v>
-      </c>
+      <c r="K94" s="20"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A95" s="41"/>
+      <c r="A95" s="41">
+        <v>45413</v>
+      </c>
       <c r="B95" s="20"/>
-      <c r="C95" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="C95" s="13"/>
       <c r="D95" s="40"/>
       <c r="E95" s="9"/>
       <c r="F95" s="20"/>
-      <c r="G95" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G95" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H95" s="40"/>
       <c r="I95" s="9"/>
@@ -3207,44 +3508,34 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="41">
-        <v>44848</v>
-      </c>
-      <c r="B96" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C96" s="13">
-        <v>1.25</v>
-      </c>
+        <v>45444</v>
+      </c>
+      <c r="B96" s="20"/>
+      <c r="C96" s="13"/>
       <c r="D96" s="40"/>
       <c r="E96" s="9"/>
       <c r="F96" s="20"/>
-      <c r="G96" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
-      </c>
-      <c r="H96" s="40">
-        <v>1</v>
-      </c>
+      <c r="G96" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H96" s="40"/>
       <c r="I96" s="9"/>
       <c r="J96" s="11"/>
-      <c r="K96" s="48">
-        <v>44848</v>
-      </c>
+      <c r="K96" s="20"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="41">
-        <v>44866</v>
+        <v>45474</v>
       </c>
       <c r="B97" s="20"/>
-      <c r="C97" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="C97" s="13"/>
       <c r="D97" s="40"/>
       <c r="E97" s="9"/>
       <c r="F97" s="20"/>
-      <c r="G97" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G97" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H97" s="40"/>
       <c r="I97" s="9"/>
@@ -3253,39 +3544,33 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="41">
-        <v>44896</v>
-      </c>
-      <c r="B98" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C98" s="13">
-        <v>1.25</v>
-      </c>
-      <c r="D98" s="40">
-        <v>3</v>
-      </c>
+        <v>45505</v>
+      </c>
+      <c r="B98" s="20"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="40"/>
       <c r="E98" s="9"/>
       <c r="F98" s="20"/>
-      <c r="G98" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G98" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H98" s="40"/>
       <c r="I98" s="9"/>
       <c r="J98" s="11"/>
-      <c r="K98" s="20" t="s">
-        <v>67</v>
-      </c>
+      <c r="K98" s="20"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A99" s="41"/>
+      <c r="A99" s="41">
+        <v>45536</v>
+      </c>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
       <c r="D99" s="40"/>
       <c r="E99" s="9"/>
       <c r="F99" s="20"/>
       <c r="G99" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H99" s="40"/>
@@ -3294,14 +3579,16 @@
       <c r="K99" s="20"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A100" s="41"/>
+      <c r="A100" s="41">
+        <v>45566</v>
+      </c>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
       <c r="D100" s="40"/>
       <c r="E100" s="9"/>
       <c r="F100" s="20"/>
       <c r="G100" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H100" s="40"/>
@@ -3310,14 +3597,16 @@
       <c r="K100" s="20"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A101" s="41"/>
+      <c r="A101" s="41">
+        <v>45597</v>
+      </c>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
       <c r="D101" s="40"/>
       <c r="E101" s="9"/>
       <c r="F101" s="20"/>
       <c r="G101" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H101" s="40"/>
@@ -3333,7 +3622,7 @@
       <c r="E102" s="9"/>
       <c r="F102" s="20"/>
       <c r="G102" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H102" s="40"/>
@@ -3349,7 +3638,7 @@
       <c r="E103" s="9"/>
       <c r="F103" s="20"/>
       <c r="G103" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H103" s="40"/>
@@ -3365,7 +3654,7 @@
       <c r="E104" s="9"/>
       <c r="F104" s="20"/>
       <c r="G104" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H104" s="40"/>
@@ -3381,7 +3670,7 @@
       <c r="E105" s="9"/>
       <c r="F105" s="20"/>
       <c r="G105" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H105" s="40"/>
@@ -3397,7 +3686,7 @@
       <c r="E106" s="9"/>
       <c r="F106" s="20"/>
       <c r="G106" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H106" s="40"/>
@@ -3413,7 +3702,7 @@
       <c r="E107" s="9"/>
       <c r="F107" s="20"/>
       <c r="G107" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H107" s="40"/>
@@ -3429,7 +3718,7 @@
       <c r="E108" s="9"/>
       <c r="F108" s="20"/>
       <c r="G108" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
       <c r="H108" s="40"/>
@@ -3438,356 +3727,1368 @@
       <c r="K108" s="20"/>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A109" s="41"/>
-      <c r="B109" s="20"/>
-      <c r="C109" s="13"/>
-      <c r="D109" s="40"/>
+      <c r="A109" s="42"/>
+      <c r="B109" s="15"/>
+      <c r="C109" s="43"/>
+      <c r="D109" s="44"/>
       <c r="E109" s="9"/>
-      <c r="F109" s="20"/>
-      <c r="G109" s="13" t="str">
+      <c r="F109" s="15"/>
+      <c r="G109" s="43" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H109" s="44"/>
+      <c r="I109" s="9"/>
+      <c r="J109" s="12"/>
+      <c r="K109" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="89" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"-,Bold"&amp;12REPUBLIC OF THE PHILIPPINES
+CITY OF TAGAYTAY
+EMPLOYEE'S LEAVE CARD</oddHeader>
+    <oddFooter>&amp;L
+PREPARED BY: ___________________
+DATE: &amp;D, &amp;T&amp;C
+CERTIFIED CORRECT BY: &amp;UALMA A. MALABANAN&amp;U
+                                   HRMO&amp;RPage &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:K67"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3696" topLeftCell="A19" activePane="bottomLeft"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="49"/>
+      <c r="D2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="25"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="54"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="26"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="49"/>
+      <c r="D4" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="26"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="51"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="H5" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="27"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
+      <c r="B9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="13">
+        <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
+        <v>0.45400000000000018</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H109" s="40"/>
-      <c r="I109" s="9"/>
-      <c r="J109" s="11"/>
-      <c r="K109" s="20"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A110" s="41"/>
-      <c r="B110" s="20"/>
-      <c r="C110" s="13"/>
-      <c r="D110" s="40"/>
-      <c r="E110" s="9"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="13" t="str">
+      <c r="H9" s="11"/>
+      <c r="I9" s="13">
+        <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
+        <v>19.625</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H110" s="40"/>
-      <c r="I110" s="9"/>
-      <c r="J110" s="11"/>
-      <c r="K110" s="20"/>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A111" s="41"/>
-      <c r="B111" s="20"/>
-      <c r="C111" s="13"/>
-      <c r="D111" s="40"/>
-      <c r="E111" s="9"/>
-      <c r="F111" s="20"/>
-      <c r="G111" s="13" t="str">
+      <c r="H10" s="40"/>
+      <c r="I10" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="41">
+        <v>43101</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H111" s="40"/>
-      <c r="I111" s="9"/>
-      <c r="J111" s="11"/>
-      <c r="K111" s="20"/>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A112" s="41"/>
-      <c r="B112" s="20"/>
-      <c r="C112" s="13"/>
-      <c r="D112" s="40"/>
-      <c r="E112" s="9"/>
-      <c r="F112" s="20"/>
-      <c r="G112" s="13" t="str">
+      <c r="H11" s="40">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="48">
+        <v>43133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="41">
+        <v>43132</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H112" s="40"/>
-      <c r="I112" s="9"/>
-      <c r="J112" s="11"/>
-      <c r="K112" s="20"/>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A113" s="41"/>
-      <c r="B113" s="20"/>
-      <c r="C113" s="13"/>
-      <c r="D113" s="40"/>
-      <c r="E113" s="9"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="13" t="str">
+      <c r="H12" s="40"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="48">
+        <v>43159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="41">
+        <v>43313</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H113" s="40"/>
-      <c r="I113" s="9"/>
-      <c r="J113" s="11"/>
-      <c r="K113" s="20"/>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A114" s="41"/>
-      <c r="B114" s="20"/>
-      <c r="C114" s="13"/>
-      <c r="D114" s="40"/>
-      <c r="E114" s="9"/>
-      <c r="F114" s="20"/>
-      <c r="G114" s="13" t="str">
+      <c r="H13" s="40">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="48">
+        <v>43313</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="41">
+        <v>43344</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H114" s="40"/>
-      <c r="I114" s="9"/>
-      <c r="J114" s="11"/>
-      <c r="K114" s="20"/>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A115" s="41"/>
-      <c r="B115" s="20"/>
-      <c r="C115" s="13"/>
-      <c r="D115" s="40"/>
-      <c r="E115" s="9"/>
-      <c r="F115" s="20"/>
-      <c r="G115" s="13" t="str">
+      <c r="H14" s="40"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="48">
+        <v>43356</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="41"/>
+      <c r="B15" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H115" s="40"/>
-      <c r="I115" s="9"/>
-      <c r="J115" s="11"/>
-      <c r="K115" s="20"/>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A116" s="41"/>
-      <c r="B116" s="20"/>
-      <c r="C116" s="13"/>
-      <c r="D116" s="40"/>
-      <c r="E116" s="9"/>
-      <c r="F116" s="20"/>
-      <c r="G116" s="13" t="str">
+      <c r="H15" s="40"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="48">
+        <v>43353</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H116" s="40"/>
-      <c r="I116" s="9"/>
-      <c r="J116" s="11"/>
-      <c r="K116" s="20"/>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A117" s="41"/>
-      <c r="B117" s="20"/>
-      <c r="C117" s="13"/>
-      <c r="D117" s="40"/>
-      <c r="E117" s="9"/>
-      <c r="F117" s="20"/>
-      <c r="G117" s="13" t="str">
+      <c r="H16" s="40"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="41">
+        <v>43647</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H117" s="40"/>
-      <c r="I117" s="9"/>
-      <c r="J117" s="11"/>
-      <c r="K117" s="20"/>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A118" s="41"/>
-      <c r="B118" s="20"/>
-      <c r="C118" s="13"/>
-      <c r="D118" s="40"/>
-      <c r="E118" s="9"/>
-      <c r="F118" s="20"/>
-      <c r="G118" s="13" t="str">
+      <c r="H17" s="40"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="48">
+        <v>43655</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="41">
+        <v>43709</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H118" s="40"/>
-      <c r="I118" s="9"/>
-      <c r="J118" s="11"/>
-      <c r="K118" s="20"/>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A119" s="41"/>
-      <c r="B119" s="20"/>
-      <c r="C119" s="13"/>
-      <c r="D119" s="40"/>
-      <c r="E119" s="9"/>
-      <c r="F119" s="20"/>
-      <c r="G119" s="13" t="str">
+      <c r="H18" s="40"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H119" s="40"/>
-      <c r="I119" s="9"/>
-      <c r="J119" s="11"/>
-      <c r="K119" s="20"/>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A120" s="41"/>
-      <c r="B120" s="20"/>
-      <c r="C120" s="13"/>
-      <c r="D120" s="40"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="20"/>
-      <c r="G120" s="13" t="str">
+      <c r="H19" s="40"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="41">
+        <v>43831</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H120" s="40"/>
-      <c r="I120" s="9"/>
-      <c r="J120" s="11"/>
-      <c r="K120" s="20"/>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A121" s="41"/>
-      <c r="B121" s="20"/>
-      <c r="C121" s="13"/>
-      <c r="D121" s="40"/>
-      <c r="E121" s="9"/>
-      <c r="F121" s="20"/>
-      <c r="G121" s="13" t="str">
+      <c r="H20" s="40"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="48">
+        <v>43847</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="41">
+        <v>43862</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H121" s="40"/>
-      <c r="I121" s="9"/>
-      <c r="J121" s="11"/>
-      <c r="K121" s="20"/>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A122" s="41"/>
-      <c r="B122" s="20"/>
-      <c r="C122" s="13"/>
-      <c r="D122" s="40"/>
-      <c r="E122" s="9"/>
-      <c r="F122" s="20"/>
-      <c r="G122" s="13" t="str">
+      <c r="H21" s="40"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="48">
+        <v>43889</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="41">
+        <v>44075</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H122" s="40"/>
-      <c r="I122" s="9"/>
-      <c r="J122" s="11"/>
-      <c r="K122" s="20"/>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A123" s="41"/>
-      <c r="B123" s="20"/>
-      <c r="C123" s="13"/>
-      <c r="D123" s="40"/>
-      <c r="E123" s="9"/>
-      <c r="F123" s="20"/>
-      <c r="G123" s="13" t="str">
+      <c r="H22" s="40"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="48">
+        <v>44088</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H123" s="40"/>
-      <c r="I123" s="9"/>
-      <c r="J123" s="11"/>
-      <c r="K123" s="20"/>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A124" s="41"/>
-      <c r="B124" s="20"/>
-      <c r="C124" s="13"/>
-      <c r="D124" s="40"/>
-      <c r="E124" s="9"/>
-      <c r="F124" s="20"/>
-      <c r="G124" s="13" t="str">
+      <c r="H23" s="40"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="20"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="41">
+        <v>44409</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H124" s="40"/>
-      <c r="I124" s="9"/>
-      <c r="J124" s="11"/>
-      <c r="K124" s="20"/>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A125" s="41"/>
-      <c r="B125" s="20"/>
-      <c r="C125" s="13"/>
-      <c r="D125" s="40"/>
-      <c r="E125" s="9"/>
-      <c r="F125" s="20"/>
-      <c r="G125" s="13" t="str">
+      <c r="H24" s="40"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H125" s="40"/>
-      <c r="I125" s="9"/>
-      <c r="J125" s="11"/>
-      <c r="K125" s="20"/>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A126" s="41"/>
-      <c r="B126" s="20"/>
-      <c r="C126" s="13"/>
-      <c r="D126" s="40"/>
-      <c r="E126" s="9"/>
-      <c r="F126" s="20"/>
-      <c r="G126" s="13" t="str">
+      <c r="H25" s="40"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="20"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="41">
+        <v>44713</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="40">
+        <v>1</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H126" s="40"/>
-      <c r="I126" s="9"/>
-      <c r="J126" s="11"/>
-      <c r="K126" s="20"/>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A127" s="41"/>
-      <c r="B127" s="20"/>
-      <c r="C127" s="13"/>
-      <c r="D127" s="40"/>
-      <c r="E127" s="9"/>
-      <c r="F127" s="20"/>
-      <c r="G127" s="13" t="str">
+      <c r="H26" s="40"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="48">
+        <v>44718</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="41"/>
+      <c r="B27" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="40">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H127" s="40"/>
-      <c r="I127" s="9"/>
-      <c r="J127" s="11"/>
-      <c r="K127" s="20"/>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A128" s="41"/>
-      <c r="B128" s="20"/>
-      <c r="C128" s="13"/>
-      <c r="D128" s="40"/>
-      <c r="E128" s="9"/>
-      <c r="F128" s="20"/>
-      <c r="G128" s="13" t="str">
+      <c r="H27" s="40"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="48">
+        <v>44729</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="41">
+        <v>44743</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H128" s="40"/>
-      <c r="I128" s="9"/>
-      <c r="J128" s="11"/>
-      <c r="K128" s="20"/>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A129" s="41"/>
-      <c r="B129" s="20"/>
-      <c r="C129" s="13"/>
-      <c r="D129" s="40"/>
-      <c r="E129" s="9"/>
-      <c r="F129" s="20"/>
-      <c r="G129" s="13" t="str">
+      <c r="H28" s="40"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="41"/>
+      <c r="B29" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="40">
+        <v>1</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H129" s="40"/>
-      <c r="I129" s="9"/>
-      <c r="J129" s="11"/>
-      <c r="K129" s="20"/>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A130" s="42"/>
-      <c r="B130" s="15"/>
-      <c r="C130" s="43"/>
-      <c r="D130" s="44"/>
-      <c r="E130" s="9"/>
-      <c r="F130" s="15"/>
-      <c r="G130" s="43" t="str">
+      <c r="H29" s="40"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="48">
+        <v>44769</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="41">
+        <v>44774</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H130" s="44"/>
-      <c r="I130" s="9"/>
-      <c r="J130" s="12"/>
-      <c r="K130" s="15"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="48">
+        <v>44793</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="41"/>
+      <c r="B31" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H31" s="40"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="48">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="41"/>
+      <c r="B32" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H32" s="40">
+        <v>1</v>
+      </c>
+      <c r="I32" s="9"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="48">
+        <v>44795</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="41">
+        <v>44805</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H33" s="40">
+        <v>1</v>
+      </c>
+      <c r="I33" s="9"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="48">
+        <v>44820</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="41">
+        <v>44848</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H34" s="40">
+        <v>1</v>
+      </c>
+      <c r="I34" s="9"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="48">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="41">
+        <v>44866</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H35" s="40">
+        <v>1</v>
+      </c>
+      <c r="I35" s="9"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="48">
+        <v>44886</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="20"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H36" s="40"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="20"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="41">
+        <v>44927</v>
+      </c>
+      <c r="B37" s="20"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H37" s="40"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="20"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="41">
+        <v>44958</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H38" s="40"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="20"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="41">
+        <v>44986</v>
+      </c>
+      <c r="B39" s="20"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H39" s="40"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="20"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="41">
+        <v>45017</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H40" s="40"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="20"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="41">
+        <v>45047</v>
+      </c>
+      <c r="B41" s="20"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H41" s="40"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="20"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="41">
+        <v>45078</v>
+      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H42" s="40"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="20"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="41">
+        <v>45108</v>
+      </c>
+      <c r="B43" s="20"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H43" s="40"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="20"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="41">
+        <v>45139</v>
+      </c>
+      <c r="B44" s="20"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H44" s="40"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="20"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="41">
+        <v>45170</v>
+      </c>
+      <c r="B45" s="20"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H45" s="40"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="20"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="41">
+        <v>45200</v>
+      </c>
+      <c r="B46" s="20"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H46" s="40"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="20"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="41">
+        <v>45231</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H47" s="40"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="20"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="41">
+        <v>45261</v>
+      </c>
+      <c r="B48" s="20"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H48" s="40"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="20"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="41">
+        <v>45292</v>
+      </c>
+      <c r="B49" s="20"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H49" s="40"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="20"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="41">
+        <v>45323</v>
+      </c>
+      <c r="B50" s="20"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H50" s="40"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="20"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="41">
+        <v>45352</v>
+      </c>
+      <c r="B51" s="20"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H51" s="40"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="20"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="41">
+        <v>45383</v>
+      </c>
+      <c r="B52" s="20"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H52" s="40"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="20"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="41">
+        <v>45413</v>
+      </c>
+      <c r="B53" s="20"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H53" s="40"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="20"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="41">
+        <v>45444</v>
+      </c>
+      <c r="B54" s="20"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H54" s="40"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="20"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="41">
+        <v>45474</v>
+      </c>
+      <c r="B55" s="20"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H55" s="40"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="20"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" s="41">
+        <v>45505</v>
+      </c>
+      <c r="B56" s="20"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H56" s="40"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="20"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" s="41">
+        <v>45536</v>
+      </c>
+      <c r="B57" s="20"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H57" s="40"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="20"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" s="41">
+        <v>45566</v>
+      </c>
+      <c r="B58" s="20"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H58" s="40"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="20"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" s="41">
+        <v>45597</v>
+      </c>
+      <c r="B59" s="20"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H59" s="40"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="20"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" s="41"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H60" s="40"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="20"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" s="41"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H61" s="40"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="20"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="41"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H62" s="40"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="20"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="41"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H63" s="40"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="20"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" s="41"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H64" s="40"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="20"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" s="41"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H65" s="40"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="20"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="41"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H66" s="40"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="20"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" s="42"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="43"/>
+      <c r="D67" s="44"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="43" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H67" s="44"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="12"/>
+      <c r="K67" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3804,10 +5105,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{3C67B38A-DE91-4BA1-85D0-F5C61D6395E6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{C9F25C0C-606E-415B-87B4-B098DE141EB5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3829,8 +5130,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB8F789-193C-43F9-8D48-B0DEE5C76ADA}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3839,8 +5140,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Update Leave Card 5/18/2023 4:35 PM
</commit_message>
<xml_diff>
--- a/ANGCAYA, JENNY ROSE.xlsx
+++ b/ANGCAYA, JENNY ROSE.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVECARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-JHL336T\Users\ASUS\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CA937C-2BDA-4541-909F-50BD538D9058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="2017 LEAVE BALANCE" sheetId="4" r:id="rId1"/>
@@ -27,7 +26,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE BALANCE'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="74">
   <si>
     <t>PERIOD</t>
   </si>
@@ -253,12 +252,18 @@
   </si>
   <si>
     <t>2/20,21/2023</t>
+  </si>
+  <si>
+    <t>SL(2-0-0)</t>
+  </si>
+  <si>
+    <t>3/31,4/3/2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -633,17 +638,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -653,6 +655,9 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1181,25 +1186,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K109" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K109" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
+    <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="21">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="17">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1211,25 +1216,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:K67" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K67" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1536,34 +1541,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3696" topLeftCell="A79" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A73" activePane="bottomLeft"/>
       <selection activeCell="I10" sqref="I10"/>
-      <selection pane="bottomLeft" activeCell="B81" sqref="B81"/>
+      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -1575,16 +1580,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="51"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -1593,16 +1598,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="50"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -1613,16 +1618,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -1630,7 +1635,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -1643,24 +1648,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52" t="s">
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -1695,7 +1700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -1704,7 +1709,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])</f>
-        <v>43.5</v>
+        <v>46</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -1714,12 +1719,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])</f>
-        <v>77.5</v>
+        <v>78</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>45</v>
       </c>
@@ -1741,7 +1746,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="41">
         <v>43101</v>
       </c>
@@ -1761,7 +1766,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="48"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="41">
         <v>43132</v>
       </c>
@@ -1785,7 +1790,7 @@
         <v>43159</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="41">
         <v>43160</v>
       </c>
@@ -1805,7 +1810,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="41">
         <v>43191</v>
       </c>
@@ -1825,7 +1830,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="41">
         <v>43221</v>
       </c>
@@ -1845,7 +1850,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>43252</v>
       </c>
@@ -1865,7 +1870,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="41">
         <v>43282</v>
       </c>
@@ -1885,7 +1890,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="41">
         <v>43313</v>
       </c>
@@ -1905,7 +1910,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="48"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="41">
         <v>43344</v>
       </c>
@@ -1929,7 +1934,7 @@
         <v>43356</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="41">
         <v>43374</v>
       </c>
@@ -1949,7 +1954,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="41">
         <v>43405</v>
       </c>
@@ -1975,7 +1980,7 @@
         <v>43427</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="41">
         <v>43435</v>
       </c>
@@ -2001,7 +2006,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>
       <c r="B23" s="20" t="s">
         <v>48</v>
@@ -2021,7 +2026,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="47" t="s">
         <v>51</v>
       </c>
@@ -2039,7 +2044,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="41">
         <v>43466</v>
       </c>
@@ -2059,7 +2064,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="41">
         <v>43497</v>
       </c>
@@ -2079,7 +2084,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="41">
         <v>43525</v>
       </c>
@@ -2099,7 +2104,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="41">
         <v>43556</v>
       </c>
@@ -2119,7 +2124,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="41">
         <v>43586</v>
       </c>
@@ -2139,7 +2144,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="41">
         <v>43617</v>
       </c>
@@ -2159,7 +2164,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="41">
         <v>43647</v>
       </c>
@@ -2183,7 +2188,7 @@
         <v>43655</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="41">
         <v>43678</v>
       </c>
@@ -2203,7 +2208,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="41">
         <v>43709</v>
       </c>
@@ -2227,7 +2232,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="41">
         <v>43739</v>
       </c>
@@ -2249,7 +2254,7 @@
         <v>43788</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="41">
         <v>43770</v>
       </c>
@@ -2273,7 +2278,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="41">
         <v>43800</v>
       </c>
@@ -2299,7 +2304,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="47" t="s">
         <v>44</v>
       </c>
@@ -2317,7 +2322,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="41">
         <v>43831</v>
       </c>
@@ -2337,7 +2342,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="48"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="41">
         <v>43862</v>
       </c>
@@ -2357,7 +2362,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="48"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="41">
         <v>43891</v>
       </c>
@@ -2377,7 +2382,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="41">
         <f>EDATE(A40,1)</f>
         <v>43922</v>
@@ -2398,7 +2403,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="41">
         <f t="shared" ref="A42:A45" si="0">EDATE(A41,1)</f>
         <v>43952</v>
@@ -2419,7 +2424,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="41">
         <f t="shared" si="0"/>
         <v>43983</v>
@@ -2440,7 +2445,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="41">
         <f t="shared" si="0"/>
         <v>44013</v>
@@ -2461,7 +2466,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="41">
         <f t="shared" si="0"/>
         <v>44044</v>
@@ -2482,7 +2487,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="41">
         <v>44075</v>
       </c>
@@ -2502,7 +2507,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="48"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="41">
         <v>44105</v>
       </c>
@@ -2522,7 +2527,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="41">
         <v>44136</v>
       </c>
@@ -2542,7 +2547,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="41">
         <v>44166</v>
       </c>
@@ -2566,7 +2571,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="47" t="s">
         <v>58</v>
       </c>
@@ -2584,7 +2589,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="41">
         <v>44197</v>
       </c>
@@ -2604,7 +2609,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="41">
         <f>EDATE(A51,1)</f>
         <v>44228</v>
@@ -2625,7 +2630,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="41">
         <f t="shared" ref="A53:A58" si="1">EDATE(A52,1)</f>
         <v>44256</v>
@@ -2646,7 +2651,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="41">
         <f t="shared" si="1"/>
         <v>44287</v>
@@ -2667,7 +2672,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="41">
         <f t="shared" si="1"/>
         <v>44317</v>
@@ -2688,7 +2693,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="41">
         <f t="shared" si="1"/>
         <v>44348</v>
@@ -2709,7 +2714,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="41">
         <f t="shared" si="1"/>
         <v>44378</v>
@@ -2730,7 +2735,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="41">
         <f t="shared" si="1"/>
         <v>44409</v>
@@ -2751,7 +2756,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="41">
         <v>44440</v>
       </c>
@@ -2771,7 +2776,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="41">
         <v>44470</v>
       </c>
@@ -2791,7 +2796,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="41">
         <v>44501</v>
       </c>
@@ -2817,7 +2822,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="41">
         <v>44531</v>
       </c>
@@ -2843,7 +2848,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="41"/>
       <c r="B63" s="20" t="s">
         <v>64</v>
@@ -2865,7 +2870,7 @@
         <v>44266</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="47" t="s">
         <v>65</v>
       </c>
@@ -2883,7 +2888,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="41">
         <v>44562</v>
       </c>
@@ -2903,7 +2908,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="41">
         <f>EDATE(A65,1)</f>
         <v>44593</v>
@@ -2924,7 +2929,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="41">
         <f t="shared" ref="A67:A70" si="2">EDATE(A66,1)</f>
         <v>44621</v>
@@ -2945,7 +2950,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="41">
         <f t="shared" si="2"/>
         <v>44652</v>
@@ -2966,7 +2971,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="41">
         <f t="shared" si="2"/>
         <v>44682</v>
@@ -2987,7 +2992,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="41">
         <f t="shared" si="2"/>
         <v>44713</v>
@@ -3014,7 +3019,7 @@
         <v>44718</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="41"/>
       <c r="B71" s="20" t="s">
         <v>64</v>
@@ -3036,7 +3041,7 @@
         <v>44729</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="41">
         <v>44743</v>
       </c>
@@ -3062,7 +3067,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="41">
         <v>44774</v>
       </c>
@@ -3082,7 +3087,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="48"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="41">
         <v>44805</v>
       </c>
@@ -3102,7 +3107,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="48"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="41">
         <v>44848</v>
       </c>
@@ -3122,7 +3127,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="48"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="41">
         <v>44866</v>
       </c>
@@ -3148,7 +3153,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="41">
         <v>44896</v>
       </c>
@@ -3174,7 +3179,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="47" t="s">
         <v>68</v>
       </c>
@@ -3192,7 +3197,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="41">
         <v>44927</v>
       </c>
@@ -3212,7 +3217,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="41">
         <v>44958</v>
       </c>
@@ -3236,43 +3241,53 @@
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="41">
         <v>44986</v>
       </c>
       <c r="B81" s="20"/>
-      <c r="C81" s="13"/>
+      <c r="C81" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D81" s="40"/>
       <c r="E81" s="9"/>
       <c r="F81" s="20"/>
-      <c r="G81" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G81" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H81" s="40"/>
       <c r="I81" s="9"/>
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="41">
         <v>45017</v>
       </c>
-      <c r="B82" s="20"/>
-      <c r="C82" s="13"/>
+      <c r="B82" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C82" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D82" s="40"/>
       <c r="E82" s="9"/>
       <c r="F82" s="20"/>
-      <c r="G82" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H82" s="40"/>
+      <c r="G82" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H82" s="40">
+        <v>2</v>
+      </c>
       <c r="I82" s="9"/>
       <c r="J82" s="11"/>
-      <c r="K82" s="20"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K82" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="41">
         <v>45047</v>
       </c>
@@ -3290,7 +3305,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="41">
         <v>45078</v>
       </c>
@@ -3308,7 +3323,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="41">
         <v>45108</v>
       </c>
@@ -3326,7 +3341,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="41">
         <v>45139</v>
       </c>
@@ -3344,7 +3359,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="41">
         <v>45170</v>
       </c>
@@ -3362,7 +3377,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="41">
         <v>45200</v>
       </c>
@@ -3380,7 +3395,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="41">
         <v>45231</v>
       </c>
@@ -3398,7 +3413,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="41">
         <v>45261</v>
       </c>
@@ -3416,7 +3431,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="41">
         <v>45292</v>
       </c>
@@ -3434,7 +3449,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="41">
         <v>45323</v>
       </c>
@@ -3452,7 +3467,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="41">
         <v>45352</v>
       </c>
@@ -3470,7 +3485,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="41">
         <v>45383</v>
       </c>
@@ -3488,7 +3503,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="41">
         <v>45413</v>
       </c>
@@ -3506,7 +3521,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="41">
         <v>45444</v>
       </c>
@@ -3524,7 +3539,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="41">
         <v>45474</v>
       </c>
@@ -3542,7 +3557,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="41">
         <v>45505</v>
       </c>
@@ -3560,7 +3575,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="41">
         <v>45536</v>
       </c>
@@ -3578,7 +3593,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="41">
         <v>45566</v>
       </c>
@@ -3596,7 +3611,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="41">
         <v>45597</v>
       </c>
@@ -3614,7 +3629,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="41"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -3630,7 +3645,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="41"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -3646,7 +3661,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="41"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -3662,7 +3677,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="41"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -3678,7 +3693,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="41"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -3694,7 +3709,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="41"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -3710,7 +3725,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="41"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -3726,7 +3741,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="42"/>
       <c r="B109" s="15"/>
       <c r="C109" s="43"/>
@@ -3744,23 +3759,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3783,34 +3798,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K67"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3696" topLeftCell="A19" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A19" activePane="bottomLeft"/>
       <selection activeCell="B4" sqref="B4:C4"/>
       <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -3822,16 +3837,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="51"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -3840,16 +3855,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="50"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -3860,16 +3875,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -3877,7 +3892,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -3890,24 +3905,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52" t="s">
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -3942,7 +3957,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -3966,7 +3981,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>45</v>
       </c>
@@ -3988,7 +4003,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="41">
         <v>43101</v>
       </c>
@@ -4012,7 +4027,7 @@
         <v>43133</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="41">
         <v>43132</v>
       </c>
@@ -4034,7 +4049,7 @@
         <v>43159</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="41">
         <v>43313</v>
       </c>
@@ -4058,7 +4073,7 @@
         <v>43313</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="41">
         <v>43344</v>
       </c>
@@ -4080,7 +4095,7 @@
         <v>43356</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="41"/>
       <c r="B15" s="20" t="s">
         <v>47</v>
@@ -4100,7 +4115,7 @@
         <v>43353</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
         <v>51</v>
       </c>
@@ -4118,7 +4133,7 @@
       <c r="J16" s="11"/>
       <c r="K16" s="20"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="41">
         <v>43647</v>
       </c>
@@ -4140,7 +4155,7 @@
         <v>43655</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="41">
         <v>43709</v>
       </c>
@@ -4162,7 +4177,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="47" t="s">
         <v>44</v>
       </c>
@@ -4180,7 +4195,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="41">
         <v>43831</v>
       </c>
@@ -4202,7 +4217,7 @@
         <v>43847</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="41">
         <v>43862</v>
       </c>
@@ -4224,7 +4239,7 @@
         <v>43889</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="41">
         <v>44075</v>
       </c>
@@ -4246,7 +4261,7 @@
         <v>44088</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
         <v>58</v>
       </c>
@@ -4264,7 +4279,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="41">
         <v>44409</v>
       </c>
@@ -4286,7 +4301,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="47" t="s">
         <v>65</v>
       </c>
@@ -4304,7 +4319,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="41">
         <v>44713</v>
       </c>
@@ -4328,7 +4343,7 @@
         <v>44718</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
       <c r="B27" s="20" t="s">
         <v>64</v>
@@ -4350,7 +4365,7 @@
         <v>44729</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="41">
         <v>44743</v>
       </c>
@@ -4372,7 +4387,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="41"/>
       <c r="B29" s="20" t="s">
         <v>64</v>
@@ -4394,7 +4409,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="41">
         <v>44774</v>
       </c>
@@ -4416,7 +4431,7 @@
         <v>44793</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="41"/>
       <c r="B31" s="20" t="s">
         <v>47</v>
@@ -4436,7 +4451,7 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="41"/>
       <c r="B32" s="20" t="s">
         <v>46</v>
@@ -4458,7 +4473,7 @@
         <v>44795</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="41">
         <v>44805</v>
       </c>
@@ -4482,7 +4497,7 @@
         <v>44820</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="41">
         <v>44848</v>
       </c>
@@ -4506,7 +4521,7 @@
         <v>44848</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="41">
         <v>44866</v>
       </c>
@@ -4530,7 +4545,7 @@
         <v>44886</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="47" t="s">
         <v>68</v>
       </c>
@@ -4548,7 +4563,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="41">
         <v>44927</v>
       </c>
@@ -4566,7 +4581,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="41">
         <v>44958</v>
       </c>
@@ -4584,7 +4599,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="41">
         <v>44986</v>
       </c>
@@ -4602,7 +4617,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="41">
         <v>45017</v>
       </c>
@@ -4620,7 +4635,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="41">
         <v>45047</v>
       </c>
@@ -4638,7 +4653,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="41">
         <v>45078</v>
       </c>
@@ -4656,7 +4671,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="41">
         <v>45108</v>
       </c>
@@ -4674,7 +4689,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="41">
         <v>45139</v>
       </c>
@@ -4692,7 +4707,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="41">
         <v>45170</v>
       </c>
@@ -4710,7 +4725,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="41">
         <v>45200</v>
       </c>
@@ -4728,7 +4743,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="41">
         <v>45231</v>
       </c>
@@ -4746,7 +4761,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="41">
         <v>45261</v>
       </c>
@@ -4764,7 +4779,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="41">
         <v>45292</v>
       </c>
@@ -4782,7 +4797,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="41">
         <v>45323</v>
       </c>
@@ -4800,7 +4815,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="41">
         <v>45352</v>
       </c>
@@ -4818,7 +4833,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="41">
         <v>45383</v>
       </c>
@@ -4836,7 +4851,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="41">
         <v>45413</v>
       </c>
@@ -4854,7 +4869,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="41">
         <v>45444</v>
       </c>
@@ -4872,7 +4887,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="41">
         <v>45474</v>
       </c>
@@ -4890,7 +4905,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="41">
         <v>45505</v>
       </c>
@@ -4908,7 +4923,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="41">
         <v>45536</v>
       </c>
@@ -4926,7 +4941,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="41">
         <v>45566</v>
       </c>
@@ -4944,7 +4959,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="41">
         <v>45597</v>
       </c>
@@ -4962,7 +4977,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="41"/>
       <c r="B60" s="20"/>
       <c r="C60" s="13"/>
@@ -4978,7 +4993,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="41"/>
       <c r="B61" s="20"/>
       <c r="C61" s="13"/>
@@ -4994,7 +5009,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="41"/>
       <c r="B62" s="20"/>
       <c r="C62" s="13"/>
@@ -5010,7 +5025,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="41"/>
       <c r="B63" s="20"/>
       <c r="C63" s="13"/>
@@ -5026,7 +5041,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="41"/>
       <c r="B64" s="20"/>
       <c r="C64" s="13"/>
@@ -5042,7 +5057,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="41"/>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -5058,7 +5073,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="41"/>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -5074,7 +5089,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="42"/>
       <c r="B67" s="15"/>
       <c r="C67" s="43"/>
@@ -5105,10 +5120,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5131,28 +5146,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="38" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="38" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="57" t="s">
         <v>33</v>
       </c>
@@ -5165,7 +5180,7 @@
       <c r="K1" s="58"/>
       <c r="L1" s="58"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -5194,7 +5209,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>3.4540000000000002</v>
       </c>
@@ -5218,7 +5233,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E4" s="1">
         <f>IF(E3=0,0,IF(ISBLANK(E3),"",VLOOKUP(E3,E7:F14,2)))</f>
         <v>0</v>
@@ -5233,10 +5248,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="39" t="s">
         <v>28</v>
       </c>
@@ -5256,7 +5271,7 @@
       <c r="K6" s="59"/>
       <c r="L6" s="59"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="38">
         <v>1</v>
       </c>
@@ -5282,7 +5297,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="38">
         <v>2</v>
       </c>
@@ -5308,7 +5323,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="38">
         <v>3</v>
       </c>
@@ -5334,7 +5349,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="38">
         <v>4</v>
       </c>
@@ -5360,7 +5375,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="38">
         <v>5</v>
       </c>
@@ -5386,7 +5401,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="38">
         <v>6</v>
       </c>
@@ -5412,7 +5427,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="38">
         <v>7</v>
       </c>
@@ -5438,7 +5453,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="38">
         <v>8</v>
       </c>
@@ -5464,7 +5479,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="38">
         <v>9</v>
       </c>
@@ -5484,7 +5499,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="38">
         <v>10</v>
       </c>
@@ -5504,7 +5519,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="38">
         <v>11</v>
       </c>
@@ -5524,7 +5539,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="38">
         <v>12</v>
       </c>
@@ -5545,7 +5560,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="38">
         <v>13</v>
       </c>
@@ -5566,7 +5581,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="38">
         <v>14</v>
       </c>
@@ -5587,7 +5602,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="38">
         <v>15</v>
       </c>
@@ -5608,7 +5623,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="38">
         <v>16</v>
       </c>
@@ -5629,7 +5644,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="38">
         <v>17</v>
       </c>
@@ -5650,7 +5665,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="38">
         <v>18</v>
       </c>
@@ -5671,7 +5686,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="38">
         <v>19</v>
       </c>
@@ -5692,7 +5707,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="38">
         <v>20</v>
       </c>
@@ -5713,7 +5728,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="38">
         <v>21</v>
       </c>
@@ -5734,7 +5749,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="38">
         <v>22</v>
       </c>
@@ -5755,7 +5770,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="38">
         <v>23</v>
       </c>
@@ -5776,7 +5791,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="38">
         <v>24</v>
       </c>
@@ -5797,7 +5812,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="38">
         <v>25</v>
       </c>
@@ -5818,7 +5833,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="38">
         <v>26</v>
       </c>
@@ -5839,7 +5854,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="38">
         <v>27</v>
       </c>
@@ -5860,7 +5875,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="38">
         <v>28</v>
       </c>
@@ -5881,7 +5896,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="38">
         <v>29</v>
       </c>
@@ -5902,7 +5917,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="38">
         <v>30</v>
       </c>
@@ -5923,7 +5938,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="38">
         <v>31</v>
       </c>
@@ -5944,7 +5959,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="38">
         <v>32</v>
       </c>
@@ -5953,7 +5968,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="38">
         <v>33</v>
       </c>
@@ -5962,7 +5977,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="38">
         <v>34</v>
       </c>
@@ -5971,7 +5986,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="38">
         <v>35</v>
       </c>
@@ -5980,7 +5995,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="38">
         <v>36</v>
       </c>
@@ -5989,7 +6004,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="38">
         <v>37</v>
       </c>
@@ -5998,7 +6013,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="38">
         <v>38</v>
       </c>
@@ -6007,7 +6022,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="38">
         <v>39</v>
       </c>
@@ -6016,7 +6031,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="38">
         <v>40</v>
       </c>
@@ -6025,7 +6040,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" s="38">
         <v>41</v>
       </c>
@@ -6034,7 +6049,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="38">
         <v>42</v>
       </c>
@@ -6043,7 +6058,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="38">
         <v>43</v>
       </c>
@@ -6052,7 +6067,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="38">
         <v>44</v>
       </c>
@@ -6061,7 +6076,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="38">
         <v>45</v>
       </c>
@@ -6070,7 +6085,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="38">
         <v>46</v>
       </c>
@@ -6079,7 +6094,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="38">
         <v>47</v>
       </c>
@@ -6088,7 +6103,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="38">
         <v>48</v>
       </c>
@@ -6097,7 +6112,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="38">
         <v>49</v>
       </c>
@@ -6106,7 +6121,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="38">
         <v>50</v>
       </c>
@@ -6115,7 +6130,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="38">
         <v>51</v>
       </c>
@@ -6124,7 +6139,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="38">
         <v>52</v>
       </c>
@@ -6133,7 +6148,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="38">
         <v>53</v>
       </c>
@@ -6142,7 +6157,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="38">
         <v>54</v>
       </c>
@@ -6151,7 +6166,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="38">
         <v>55</v>
       </c>
@@ -6160,7 +6175,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="38">
         <v>56</v>
       </c>
@@ -6169,7 +6184,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="38">
         <v>57</v>
       </c>
@@ -6178,7 +6193,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="38">
         <v>58</v>
       </c>
@@ -6187,7 +6202,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="38">
         <v>59</v>
       </c>
@@ -6196,7 +6211,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="38">
         <v>60</v>
       </c>
@@ -6205,7 +6220,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>